<commit_message>
Update WDI_T3_Project_Tracker   * Close out user story and wireframes task in the schedule
</commit_message>
<xml_diff>
--- a/project_docs/tracker/WDI_T3_Project_Tracker.xlsx
+++ b/project_docs/tracker/WDI_T3_Project_Tracker.xlsx
@@ -15,6 +15,7 @@
     <sheet name="WF_T3_Sign_up" sheetId="7" r:id="rId6"/>
     <sheet name="WF_T3_Password_Reset" sheetId="8" r:id="rId7"/>
     <sheet name="WF_T3_Game_board" sheetId="9" r:id="rId8"/>
+    <sheet name="dir_structure" sheetId="10" r:id="rId9"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="2">Dev_Tasklist!$1:$2</definedName>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="141">
   <si>
     <t>T3 Project Schedule</t>
   </si>
@@ -48,12 +49,6 @@
     <t>Deliverable</t>
   </si>
   <si>
-    <t>User stories</t>
-  </si>
-  <si>
-    <t>Wireframes</t>
-  </si>
-  <si>
     <t>Status</t>
   </si>
   <si>
@@ -67,9 +62,6 @@
   </si>
   <si>
     <t>Pending</t>
-  </si>
-  <si>
-    <t>In-process</t>
   </si>
   <si>
     <t>Subtasks</t>
@@ -429,6 +421,45 @@
   </si>
   <si>
     <t>Footer</t>
+  </si>
+  <si>
+    <t>Initial user stories</t>
+  </si>
+  <si>
+    <t>Initial wireframes</t>
+  </si>
+  <si>
+    <t>Completed</t>
+  </si>
+  <si>
+    <t>/.git</t>
+  </si>
+  <si>
+    <t>/assets</t>
+  </si>
+  <si>
+    <t>grunt</t>
+  </si>
+  <si>
+    <t>/lib</t>
+  </si>
+  <si>
+    <t>/node_modules</t>
+  </si>
+  <si>
+    <t>/project_docs</t>
+  </si>
+  <si>
+    <t>/spec</t>
+  </si>
+  <si>
+    <t>~/wdi/projects/t3</t>
+  </si>
+  <si>
+    <t>/scripts</t>
+  </si>
+  <si>
+    <t>/styles</t>
   </si>
 </sst>
 </file>
@@ -1015,7 +1046,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="81">
+  <cellStyleXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1097,6 +1128,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1361,7 +1393,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="81">
+  <cellStyles count="82">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1406,6 +1438,7 @@
     <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="79" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="81" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1774,7 +1807,7 @@
   <dimension ref="A1:H40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection sqref="A1:H1"/>
+      <selection activeCell="E4" sqref="E4:H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1819,13 +1852,13 @@
         <v>4</v>
       </c>
       <c r="C3" s="49" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D3" s="49" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E3" s="52" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F3" s="52"/>
       <c r="G3" s="52"/>
@@ -1836,10 +1869,10 @@
         <v>43138</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>5</v>
+        <v>128</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>12</v>
+        <v>130</v>
       </c>
       <c r="E4" s="50"/>
       <c r="F4" s="50"/>
@@ -1849,10 +1882,10 @@
     <row r="5" spans="1:8">
       <c r="A5" s="2"/>
       <c r="B5" s="1" t="s">
-        <v>6</v>
+        <v>129</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>12</v>
+        <v>130</v>
       </c>
       <c r="E5" s="50"/>
       <c r="F5" s="50"/>
@@ -1864,10 +1897,10 @@
         <v>43140</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>11</v>
       </c>
       <c r="E6" s="50"/>
       <c r="F6" s="50"/>
@@ -1879,10 +1912,10 @@
         <v>43141</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E7" s="50"/>
       <c r="F7" s="50"/>
@@ -2133,8 +2166,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F46"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection sqref="A1:E1"/>
+    <sheetView topLeftCell="A19" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2149,7 +2182,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="20">
       <c r="A1" s="51" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B1" s="51"/>
       <c r="C1" s="51"/>
@@ -2158,31 +2191,31 @@
     </row>
     <row r="2" spans="1:6" ht="18">
       <c r="A2" s="49" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B2" s="49" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C2" s="49" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D2" s="49" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E2" s="49" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F2" s="49"/>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D3" s="1" t="str">
         <f>IF(C3="Y","Active","Future")</f>
@@ -2191,13 +2224,13 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D4" s="1" t="str">
         <f t="shared" ref="D4:D30" si="0">IF(C4="Y","Active","Future")</f>
@@ -2206,13 +2239,13 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D5" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2221,13 +2254,13 @@
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D6" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2236,13 +2269,13 @@
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D7" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2251,13 +2284,13 @@
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D8" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2266,13 +2299,13 @@
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D9" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2281,13 +2314,13 @@
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D10" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2296,13 +2329,13 @@
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D11" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2311,13 +2344,13 @@
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D12" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2326,13 +2359,13 @@
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D13" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2341,13 +2374,13 @@
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D14" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2356,13 +2389,13 @@
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D15" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2371,13 +2404,13 @@
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D16" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2386,13 +2419,13 @@
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D17" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2401,13 +2434,13 @@
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D18" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2416,13 +2449,13 @@
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D19" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2431,13 +2464,13 @@
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D20" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2446,13 +2479,13 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D21" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2461,13 +2494,13 @@
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D22" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2476,13 +2509,13 @@
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D23" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2491,13 +2524,13 @@
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D24" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2506,13 +2539,13 @@
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D25" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2521,13 +2554,13 @@
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B26" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C26" s="1" t="s">
         <v>40</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="D26" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2536,13 +2569,13 @@
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D27" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2551,13 +2584,13 @@
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D28" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2566,13 +2599,13 @@
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D29" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2581,13 +2614,13 @@
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B30" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B30" s="1" t="s">
-        <v>63</v>
-      </c>
       <c r="C30" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D30" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2596,13 +2629,13 @@
     </row>
     <row r="31" spans="1:4" ht="75">
       <c r="A31" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D31" s="1" t="str">
         <f t="shared" ref="D31:D46" si="1">IF(C31="Y","Active","Future")</f>
@@ -2611,13 +2644,13 @@
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D32" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2626,13 +2659,13 @@
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D33" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2641,13 +2674,13 @@
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D34" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2656,13 +2689,13 @@
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D35" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2671,13 +2704,13 @@
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D36" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2686,13 +2719,13 @@
     </row>
     <row r="37" spans="1:4">
       <c r="A37" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D37" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2701,13 +2734,13 @@
     </row>
     <row r="38" spans="1:4">
       <c r="A38" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D38" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2716,13 +2749,13 @@
     </row>
     <row r="39" spans="1:4" ht="30">
       <c r="A39" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D39" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2731,13 +2764,13 @@
     </row>
     <row r="40" spans="1:4">
       <c r="A40" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D40" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2746,7 +2779,7 @@
     </row>
     <row r="41" spans="1:4">
       <c r="A41" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D41" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2755,7 +2788,7 @@
     </row>
     <row r="42" spans="1:4">
       <c r="A42" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D42" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2764,7 +2797,7 @@
     </row>
     <row r="43" spans="1:4">
       <c r="A43" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D43" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2773,7 +2806,7 @@
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D44" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2782,7 +2815,7 @@
     </row>
     <row r="45" spans="1:4">
       <c r="A45" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D45" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2791,7 +2824,7 @@
     </row>
     <row r="46" spans="1:4">
       <c r="A46" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D46" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2835,7 +2868,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="20">
       <c r="A1" s="51" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B1" s="51"/>
       <c r="C1" s="51"/>
@@ -2843,86 +2876,86 @@
     </row>
     <row r="2" spans="1:4" ht="18">
       <c r="A2" s="49" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B2" s="49" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C2" s="49" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D2" s="49"/>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -2959,7 +2992,7 @@
       <c r="A1" s="4"/>
       <c r="B1" s="5"/>
       <c r="C1" s="54" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D1" s="55"/>
       <c r="E1" s="56"/>
@@ -2993,19 +3026,19 @@
     <row r="4" spans="1:9">
       <c r="A4" s="9"/>
       <c r="B4" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="E4" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="F4" s="11" t="s">
         <v>78</v>
-      </c>
-      <c r="D4" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="E4" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="F4" s="11" t="s">
-        <v>81</v>
       </c>
       <c r="G4" s="10"/>
       <c r="H4" s="7"/>
@@ -3396,7 +3429,7 @@
     </row>
     <row r="40" spans="1:9">
       <c r="A40" s="60" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B40" s="61"/>
       <c r="C40" s="61"/>
@@ -3458,7 +3491,7 @@
       <c r="A1" s="4"/>
       <c r="B1" s="42"/>
       <c r="C1" s="54" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D1" s="55"/>
       <c r="E1" s="56"/>
@@ -3492,19 +3525,19 @@
     <row r="4" spans="1:9" s="8" customFormat="1" ht="45">
       <c r="A4" s="9"/>
       <c r="B4" s="40" t="s">
+        <v>74</v>
+      </c>
+      <c r="C4" s="41" t="s">
+        <v>75</v>
+      </c>
+      <c r="D4" s="41" t="s">
+        <v>112</v>
+      </c>
+      <c r="E4" s="41" t="s">
         <v>77</v>
       </c>
-      <c r="C4" s="41" t="s">
+      <c r="F4" s="41" t="s">
         <v>78</v>
-      </c>
-      <c r="D4" s="41" t="s">
-        <v>115</v>
-      </c>
-      <c r="E4" s="41" t="s">
-        <v>80</v>
-      </c>
-      <c r="F4" s="41" t="s">
-        <v>81</v>
       </c>
       <c r="G4" s="10"/>
       <c r="H4" s="7"/>
@@ -3546,12 +3579,12 @@
     <row r="8" spans="1:9" s="8" customFormat="1" ht="30">
       <c r="A8" s="9"/>
       <c r="B8" s="16" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C8" s="19"/>
       <c r="D8" s="19"/>
       <c r="E8" s="18" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="F8" s="19"/>
       <c r="G8" s="10"/>
@@ -3572,12 +3605,12 @@
     <row r="10" spans="1:9" s="8" customFormat="1" ht="45">
       <c r="A10" s="9"/>
       <c r="B10" s="16" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C10" s="19"/>
       <c r="D10" s="19"/>
       <c r="E10" s="18" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="F10" s="19"/>
       <c r="G10" s="10"/>
@@ -3609,12 +3642,12 @@
     <row r="13" spans="1:9" s="8" customFormat="1">
       <c r="A13" s="9"/>
       <c r="B13" s="23" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C13" s="19"/>
       <c r="D13" s="39"/>
       <c r="E13" s="19" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="F13" s="39"/>
       <c r="G13" s="10"/>
@@ -3635,14 +3668,14 @@
     <row r="15" spans="1:9" s="8" customFormat="1">
       <c r="A15" s="9"/>
       <c r="B15" s="23" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C15" s="19" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D15" s="39"/>
       <c r="E15" s="19" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="F15" s="39"/>
       <c r="G15" s="10"/>
@@ -3652,17 +3685,17 @@
     <row r="16" spans="1:9" s="8" customFormat="1">
       <c r="A16" s="9"/>
       <c r="B16" s="23" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C16" s="19" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D16" s="39"/>
       <c r="E16" s="19" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="F16" s="39" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="G16" s="10"/>
       <c r="H16" s="7"/>
@@ -3671,10 +3704,10 @@
     <row r="17" spans="1:9" s="8" customFormat="1">
       <c r="A17" s="9"/>
       <c r="B17" s="23" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C17" s="19" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D17" s="39"/>
       <c r="E17" s="19"/>
@@ -3686,10 +3719,10 @@
     <row r="18" spans="1:9" s="8" customFormat="1">
       <c r="A18" s="9"/>
       <c r="B18" s="23" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C18" s="19" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D18" s="39"/>
       <c r="E18" s="19"/>
@@ -3874,7 +3907,7 @@
     </row>
     <row r="35" spans="1:9" s="8" customFormat="1">
       <c r="A35" s="60" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B35" s="61"/>
       <c r="C35" s="61"/>
@@ -3934,7 +3967,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I40"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0"/>
+    <sheetView topLeftCell="A17" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
@@ -3945,7 +3978,7 @@
       <c r="A1" s="4"/>
       <c r="B1" s="5"/>
       <c r="C1" s="54" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D1" s="55"/>
       <c r="E1" s="56"/>
@@ -3979,19 +4012,19 @@
     <row r="4" spans="1:9" ht="45">
       <c r="A4" s="9"/>
       <c r="B4" s="40" t="s">
+        <v>74</v>
+      </c>
+      <c r="C4" s="41" t="s">
+        <v>75</v>
+      </c>
+      <c r="D4" s="41" t="s">
+        <v>112</v>
+      </c>
+      <c r="E4" s="41" t="s">
         <v>77</v>
       </c>
-      <c r="C4" s="41" t="s">
+      <c r="F4" s="41" t="s">
         <v>78</v>
-      </c>
-      <c r="D4" s="41" t="s">
-        <v>115</v>
-      </c>
-      <c r="E4" s="41" t="s">
-        <v>80</v>
-      </c>
-      <c r="F4" s="41" t="s">
-        <v>81</v>
       </c>
       <c r="G4" s="10"/>
       <c r="H4" s="7"/>
@@ -4024,7 +4057,7 @@
       <c r="B7" s="31"/>
       <c r="C7" s="7"/>
       <c r="D7" s="7" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="E7" s="7"/>
       <c r="F7" s="32"/>
@@ -4047,11 +4080,11 @@
       <c r="A9" s="9"/>
       <c r="B9" s="31"/>
       <c r="C9" s="7" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D9" s="7"/>
       <c r="E9" s="77" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F9" s="78"/>
       <c r="G9" s="10"/>
@@ -4062,11 +4095,11 @@
       <c r="A10" s="9"/>
       <c r="B10" s="31"/>
       <c r="C10" s="7" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D10" s="7"/>
       <c r="E10" s="77" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="F10" s="78"/>
       <c r="G10" s="10"/>
@@ -4077,11 +4110,11 @@
       <c r="A11" s="9"/>
       <c r="B11" s="31"/>
       <c r="C11" s="7" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D11" s="7"/>
       <c r="E11" s="77" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="F11" s="78"/>
       <c r="G11" s="10"/>
@@ -4103,7 +4136,7 @@
       <c r="A13" s="9"/>
       <c r="B13" s="31"/>
       <c r="C13" s="65" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="D13" s="61"/>
       <c r="E13" s="66"/>
@@ -4136,7 +4169,7 @@
     </row>
     <row r="16" spans="1:9">
       <c r="A16" s="9" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B16" s="7"/>
       <c r="C16" s="7"/>
@@ -4149,7 +4182,7 @@
     </row>
     <row r="17" spans="1:9" ht="16" thickBot="1">
       <c r="A17" s="17" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B17" s="7"/>
       <c r="C17" s="7"/>
@@ -4174,7 +4207,7 @@
     <row r="19" spans="1:9">
       <c r="A19" s="9"/>
       <c r="B19" s="67" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C19" s="68"/>
       <c r="D19" s="68"/>
@@ -4199,7 +4232,7 @@
       <c r="A21" s="9"/>
       <c r="B21" s="31"/>
       <c r="C21" s="65" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="D21" s="61"/>
       <c r="E21" s="66"/>
@@ -4241,7 +4274,7 @@
     </row>
     <row r="25" spans="1:9" ht="16" thickBot="1">
       <c r="A25" s="17" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B25" s="7"/>
       <c r="C25" s="7"/>
@@ -4266,7 +4299,7 @@
     <row r="27" spans="1:9">
       <c r="A27" s="9"/>
       <c r="B27" s="67" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C27" s="68"/>
       <c r="D27" s="68"/>
@@ -4291,7 +4324,7 @@
       <c r="A29" s="9"/>
       <c r="B29" s="31"/>
       <c r="C29" s="70" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="D29" s="71"/>
       <c r="E29" s="72"/>
@@ -4333,7 +4366,7 @@
     </row>
     <row r="33" spans="1:7" ht="16" thickBot="1">
       <c r="A33" s="17" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B33" s="7"/>
       <c r="C33" s="7"/>
@@ -4355,7 +4388,7 @@
       <c r="A35" s="9"/>
       <c r="B35" s="31"/>
       <c r="C35" s="76" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="D35" s="76"/>
       <c r="E35" s="76"/>
@@ -4366,7 +4399,7 @@
       <c r="A36" s="9"/>
       <c r="B36" s="31"/>
       <c r="C36" s="68" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="D36" s="68"/>
       <c r="E36" s="68"/>
@@ -4386,7 +4419,7 @@
       <c r="A38" s="9"/>
       <c r="B38" s="31"/>
       <c r="C38" s="70" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="D38" s="71"/>
       <c r="E38" s="72"/>
@@ -4456,7 +4489,7 @@
       <c r="A1" s="4"/>
       <c r="B1" s="5"/>
       <c r="C1" s="54" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D1" s="55"/>
       <c r="E1" s="56"/>
@@ -4490,19 +4523,19 @@
     <row r="4" spans="1:9" ht="45">
       <c r="A4" s="9"/>
       <c r="B4" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="D4" s="18" t="s">
+        <v>112</v>
+      </c>
+      <c r="E4" s="18" t="s">
         <v>77</v>
       </c>
-      <c r="C4" s="18" t="s">
+      <c r="F4" s="18" t="s">
         <v>78</v>
-      </c>
-      <c r="D4" s="18" t="s">
-        <v>115</v>
-      </c>
-      <c r="E4" s="18" t="s">
-        <v>80</v>
-      </c>
-      <c r="F4" s="18" t="s">
-        <v>81</v>
       </c>
       <c r="G4" s="10"/>
       <c r="H4" s="7"/>
@@ -4535,7 +4568,7 @@
       <c r="B7" s="31"/>
       <c r="C7" s="7"/>
       <c r="D7" s="7" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="E7" s="7"/>
       <c r="F7" s="32"/>
@@ -4557,12 +4590,12 @@
     <row r="9" spans="1:9">
       <c r="A9" s="9"/>
       <c r="B9" s="67" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C9" s="68"/>
       <c r="D9" s="79"/>
       <c r="E9" s="77" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="F9" s="78"/>
       <c r="G9" s="10"/>
@@ -4572,12 +4605,12 @@
     <row r="10" spans="1:9">
       <c r="A10" s="9"/>
       <c r="B10" s="67" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C10" s="68"/>
       <c r="D10" s="79"/>
       <c r="E10" s="77" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="F10" s="78"/>
       <c r="G10" s="10"/>
@@ -4587,12 +4620,12 @@
     <row r="11" spans="1:9">
       <c r="A11" s="9"/>
       <c r="B11" s="67" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C11" s="68"/>
       <c r="D11" s="79"/>
       <c r="E11" s="77" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="F11" s="78"/>
       <c r="G11" s="10"/>
@@ -4614,7 +4647,7 @@
       <c r="A13" s="9"/>
       <c r="B13" s="31"/>
       <c r="C13" s="65" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D13" s="61"/>
       <c r="E13" s="66"/>
@@ -4875,7 +4908,7 @@
     </row>
     <row r="38" spans="1:7">
       <c r="A38" s="60" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B38" s="61"/>
       <c r="C38" s="61"/>
@@ -4944,7 +4977,7 @@
       <c r="A1" s="4"/>
       <c r="B1" s="5"/>
       <c r="C1" s="54" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D1" s="55"/>
       <c r="E1" s="56"/>
@@ -4978,19 +5011,19 @@
     <row r="4" spans="1:9">
       <c r="A4" s="9"/>
       <c r="B4" s="18" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C4" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="D4" s="18" t="s">
+        <v>113</v>
+      </c>
+      <c r="E4" s="18" t="s">
+        <v>114</v>
+      </c>
+      <c r="F4" s="18" t="s">
         <v>78</v>
-      </c>
-      <c r="D4" s="18" t="s">
-        <v>116</v>
-      </c>
-      <c r="E4" s="18" t="s">
-        <v>117</v>
-      </c>
-      <c r="F4" s="18" t="s">
-        <v>81</v>
       </c>
       <c r="G4" s="10"/>
       <c r="H4" s="7"/>
@@ -5022,7 +5055,7 @@
       <c r="A7" s="9"/>
       <c r="B7" s="7"/>
       <c r="C7" s="68" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="D7" s="68"/>
       <c r="E7" s="68"/>
@@ -5046,13 +5079,13 @@
       <c r="A9" s="9"/>
       <c r="B9" s="7"/>
       <c r="C9" s="80" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="D9" s="83" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="E9" s="86" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="F9" s="7"/>
       <c r="G9" s="10"/>
@@ -5074,13 +5107,13 @@
       <c r="A11" s="9"/>
       <c r="B11" s="7"/>
       <c r="C11" s="81" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="D11" s="84" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="E11" s="87" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="F11" s="7"/>
       <c r="G11" s="10"/>
@@ -5102,13 +5135,13 @@
       <c r="A13" s="9"/>
       <c r="B13" s="7"/>
       <c r="C13" s="81" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="D13" s="84" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="E13" s="87" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="F13" s="7"/>
       <c r="G13" s="10"/>
@@ -5140,17 +5173,17 @@
     <row r="16" spans="1:9" ht="30">
       <c r="A16" s="9"/>
       <c r="B16" s="20" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C16" s="48" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="D16" s="7"/>
       <c r="E16" s="20" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="F16" s="45" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="G16" s="10"/>
       <c r="H16" s="7"/>
@@ -5159,14 +5192,14 @@
     <row r="17" spans="1:9" ht="30">
       <c r="A17" s="9"/>
       <c r="B17" s="46" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C17" s="24">
         <v>100</v>
       </c>
       <c r="D17" s="7"/>
       <c r="E17" s="46" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="F17" s="24">
         <v>100</v>
@@ -5178,14 +5211,14 @@
     <row r="18" spans="1:9" ht="30">
       <c r="A18" s="9"/>
       <c r="B18" s="46" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C18" s="24">
         <v>50</v>
       </c>
       <c r="D18" s="7"/>
       <c r="E18" s="46" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="F18" s="24">
         <v>50</v>
@@ -5197,14 +5230,14 @@
     <row r="19" spans="1:9">
       <c r="A19" s="9"/>
       <c r="B19" s="46" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C19" s="24">
         <v>50</v>
       </c>
       <c r="D19" s="7"/>
       <c r="E19" s="46" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="F19" s="24">
         <v>50</v>
@@ -5214,7 +5247,7 @@
     <row r="20" spans="1:9">
       <c r="A20" s="9"/>
       <c r="B20" s="25" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C20" s="47">
         <f>SUM(C18/C17)</f>
@@ -5222,7 +5255,7 @@
       </c>
       <c r="D20" s="7"/>
       <c r="E20" s="25" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="F20" s="47">
         <f>SUM(F18/F17)</f>
@@ -5376,7 +5409,7 @@
     </row>
     <row r="37" spans="1:7">
       <c r="A37" s="60" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B37" s="61"/>
       <c r="C37" s="61"/>
@@ -5434,4 +5467,80 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="B2" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="B3" t="s">
+        <v>132</v>
+      </c>
+      <c r="C3" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="B4" t="s">
+        <v>132</v>
+      </c>
+      <c r="C4" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="B5" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="B6" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="B7" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="B8" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="B9" t="s">
+        <v>137</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>